<commit_message>
generate dummies for section
</commit_message>
<xml_diff>
--- a/labels.xlsx
+++ b/labels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miamiamia/Desktop/725finalproject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miamiamia/Desktop/Econ725_finalproject_group7/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="268">
   <si>
     <t>Variables</t>
   </si>
@@ -842,6 +842,10 @@
   </si>
   <si>
     <t>season tickets dummy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of tickets</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -863,6 +867,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -872,6 +877,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1201,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD62"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1305,6 +1311,9 @@
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">

</xml_diff>